<commit_message>
added coins, upgrade, buy
fixed knight check bug
</commit_message>
<xml_diff>
--- a/PawnShop/Data/Data.xlsx
+++ b/PawnShop/Data/Data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Projects\Git\ChessUltimate\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Projects\Git\PawnShop\PawnShop\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45681196-B05E-46D0-8DF2-EC4C81513612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{73BB59C0-EE19-4574-8AA9-F1A6D2D1E5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{ECBFDE40-5963-4617-AE30-0CC7F799B5F4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{ECBFDE40-5963-4617-AE30-0CC7F799B5F4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="InitBoard_Traditional" sheetId="1" r:id="rId1"/>
+    <sheet name="InitBoard_PawnShop" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="20">
   <si>
     <t>Side</t>
   </si>
@@ -102,8 +103,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -131,8 +140,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,30 +459,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C91FE69-6ABB-49F2-B936-87082A5A3393}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26:F27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -486,7 +496,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -500,7 +510,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -514,7 +524,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -528,7 +538,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -542,7 +552,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -556,7 +566,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -570,7 +580,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -584,7 +594,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -598,7 +608,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -612,7 +622,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -626,7 +636,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -640,7 +650,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -654,7 +664,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -668,7 +678,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -682,7 +692,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -696,7 +706,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -710,7 +720,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -724,7 +734,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -738,7 +748,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -752,7 +762,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -766,7 +776,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -780,7 +790,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -794,7 +804,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -808,7 +818,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -822,7 +832,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -836,7 +846,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -850,7 +860,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -864,7 +874,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -878,7 +888,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -892,7 +902,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -906,7 +916,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -923,4 +933,62 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8720F4F8-FC20-47A3-A804-552DB139204A}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>